<commit_message>
project folder structure and settings
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/CIC_Claims_Automation_Assessment/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4622AA53-24E0-47C6-B396-B65918DC4998}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC8228C-1FCD-4CAE-AC12-90AEE860354C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,10 +196,10 @@
     <t>MaxClaimAmount</t>
   </si>
   <si>
-    <t>23-07-2025</t>
-  </si>
-  <si>
-    <t>23-07-2024</t>
+    <t>2024-07-23</t>
+  </si>
+  <si>
+    <t>2025-07-23</t>
   </si>
 </sst>
 </file>
@@ -277,10 +277,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,7 +886,7 @@
         <v>53</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -898,7 +894,7 @@
         <v>54</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3">

</xml_diff>

<commit_message>
feat(init): implement ReadClaimsData workflow and business/system exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC8228C-1FCD-4CAE-AC12-90AEE860354C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2CF2B6-A975-42F3-86D4-500CDE2A8692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -200,6 +200,106 @@
   </si>
   <si>
     <t>2025-07-23</t>
+  </si>
+  <si>
+    <t>SQLiteDBPath</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Database\claims.db</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>ClaimsData</t>
+  </si>
+  <si>
+    <t>SenderEmail</t>
+  </si>
+  <si>
+    <t>mwaimoris@outlook.com</t>
+  </si>
+  <si>
+    <t>RecipientEmail_Business</t>
+  </si>
+  <si>
+    <t>RecipientEmail_System</t>
+  </si>
+  <si>
+    <t>Subject_NoFileFound</t>
+  </si>
+  <si>
+    <t>Body_NoFileFound</t>
+  </si>
+  <si>
+    <t>Subject_EmptyFile</t>
+  </si>
+  <si>
+    <t>Body_EmptyFile</t>
+  </si>
+  <si>
+    <t>Subject_InvalidExcelFormat</t>
+  </si>
+  <si>
+    <t>Body_InvalidExcelFormat</t>
+  </si>
+  <si>
+    <t>mwaimoris@gmail.com</t>
+  </si>
+  <si>
+    <t>morismwai1@gmail.com</t>
+  </si>
+  <si>
+    <t>Missing Input File</t>
+  </si>
+  <si>
+    <t>Empty Claims File</t>
+  </si>
+  <si>
+    <t>Invalid Excel Format</t>
+  </si>
+  <si>
+    <t>Subject_SystemException</t>
+  </si>
+  <si>
+    <t>Hello,
+An exception occurred during the automation process. Please find the details below:
+Exception Source: @Source
+Exception Message: @Message
+A screenshot of the error has been attached for reference. Please see the attachment for more details.
+Thank you and have a good day,
+Robot :)</t>
+  </si>
+  <si>
+    <t>Hello,
+The automation was unable to process the file due to missing or incorrect headers in the Excel sheet. 
+Please correct the format and upload again. 
+Timestamp: @Timestamp 
+Best regards, 
+Robot :)</t>
+  </si>
+  <si>
+    <t>Hello, 
+The automation could not proceed because the claims data file is empty. 
+Please verify the data and reload the file. 
+Timestamp: @Timestamp 
+Best regards,
+Robot :)</t>
+  </si>
+  <si>
+    <t>Body_SystemException</t>
+  </si>
+  <si>
+    <t>Automation Error!</t>
+  </si>
+  <si>
+    <t>Hello,
+The automation was unable to start because the required input file was not found at path:
+@InputFilePath
+Please upload the file and notify the automation team.
+Timesstamp: @Timestamp
+Best regards,
+Robot :)</t>
   </si>
 </sst>
 </file>
@@ -251,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +362,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,16 +767,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -865,6 +966,14 @@
         <v>48</v>
       </c>
     </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>49</v>
@@ -903,6 +1012,102 @@
       </c>
       <c r="B26">
         <v>1000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="180">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="150">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="165">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="180">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(validation): add UiPath-based claim validation and Python hashing integration
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2CF2B6-A975-42F3-86D4-500CDE2A8692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A322AE96-6506-438A-A26C-0D48B1877976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -300,6 +300,24 @@
 Timesstamp: @Timestamp
 Best regards,
 Robot :)</t>
+  </si>
+  <si>
+    <t>pythonPath</t>
+  </si>
+  <si>
+    <t>C:\\Python312\\</t>
+  </si>
+  <si>
+    <t>pythonLibraryPath</t>
+  </si>
+  <si>
+    <t>C:\\Python312\\python312.dll</t>
+  </si>
+  <si>
+    <t>HashScriptPath</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Python_Scripts\hash_policyholder_id.py</t>
   </si>
 </sst>
 </file>
@@ -351,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -362,7 +380,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -820,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
@@ -1026,7 +1043,7 @@
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1034,7 +1051,7 @@
       <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1042,7 +1059,7 @@
       <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1108,6 +1125,30 @@
       </c>
       <c r="B43" s="3" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added enhanced validation logic with date normalization and decimal parsing in ValidateClaim_UiPath.xaml. Partially implemented InsertIntoSQLite.xaml with Run Command activity and static value insert test.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145DB794-E380-41C6-BBE3-4183196E896C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4287F95-FD5D-46DF-9168-4E7CD713300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -305,15 +305,9 @@
     <t>pythonPath</t>
   </si>
   <si>
-    <t>C:\\Python312\\</t>
-  </si>
-  <si>
     <t>pythonLibraryPath</t>
   </si>
   <si>
-    <t>C:\\Python312\\python312.dll</t>
-  </si>
-  <si>
     <t>HashScriptPath</t>
   </si>
   <si>
@@ -324,6 +318,21 @@
   </si>
   <si>
     <t>DbPath</t>
+  </si>
+  <si>
+    <t>C:\Python312</t>
+  </si>
+  <si>
+    <t>C:\Python312\python312.dll</t>
+  </si>
+  <si>
+    <t>SQLiteDSN</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Database\claims_encrypted.db</t>
+  </si>
+  <si>
+    <t>ClaimsAutomation</t>
   </si>
 </sst>
 </file>
@@ -702,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -763,6 +772,9 @@
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>44</v>
       </c>
@@ -790,10 +802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z49"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1138,31 +1150,39 @@
         <v>84</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30">
+      <c r="A49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>91</v>
-      </c>
       <c r="B49" s="3" t="s">
-        <v>59</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1225,10 +1245,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
feat: add Python-based claim validation and database error handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4287F95-FD5D-46DF-9168-4E7CD713300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FEFDD4-63ED-48EC-BEFF-A6EC18A09B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -333,6 +333,31 @@
   </si>
   <si>
     <t>ClaimsAutomation</t>
+  </si>
+  <si>
+    <t>ValidateScriptPath</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Python_Scripts\validate_claims.py</t>
+  </si>
+  <si>
+    <t>Subject_DatabaseError</t>
+  </si>
+  <si>
+    <t>Database Connection Error!</t>
+  </si>
+  <si>
+    <t>Body_DatabaseError</t>
+  </si>
+  <si>
+    <t>Hello,
+An error occurred while connecting to or interacting with the database. Please review the details below:
+Exception Source: @Source  
+Exception Message: @Message  
+This might be due to incorrect DSN configuration, network issues, or driver-specific errors.
+A screenshot of the error has been attached for reference.
+Thank you,  
+Robot :)</t>
   </si>
 </sst>
 </file>
@@ -711,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -802,10 +827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1145,43 +1170,67 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="225">
       <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30">
-      <c r="A47" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30">
       <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="30">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30">
+      <c r="A52" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor summary generation workflow and add success email notification
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FEFDD4-63ED-48EC-BEFF-A6EC18A09B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0257FB57-651D-4C05-AF0D-A2CE44351981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="-13500" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -172,9 +172,6 @@
     <t>ClaimsSummaryFilePath</t>
   </si>
   <si>
-    <t>Data\Output\claims_summary.xlsx</t>
-  </si>
-  <si>
     <t>ValidBranches</t>
   </si>
   <si>
@@ -200,12 +197,6 @@
   </si>
   <si>
     <t>2025-07-23</t>
-  </si>
-  <si>
-    <t>SQLiteDBPath</t>
-  </si>
-  <si>
-    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Database\claims.db</t>
   </si>
   <si>
     <t>SheetName</t>
@@ -358,6 +349,71 @@
 A screenshot of the error has been attached for reference.
 Thank you,  
 Robot :)</t>
+  </si>
+  <si>
+    <t>SQL_TotalClaimsProcessed</t>
+  </si>
+  <si>
+    <t>SQL_ValidClaimsCount</t>
+  </si>
+  <si>
+    <t>SQL_InvalidClaimsCount</t>
+  </si>
+  <si>
+    <t>SQL_ClaimTypeBreakdown</t>
+  </si>
+  <si>
+    <t>SELECT Claim_Type, COUNT(*) AS Count FROM Valid_Claims WHERE Processed_Timestamp = '@RunStart' GROUP BY Claim_Type</t>
+  </si>
+  <si>
+    <t>SQL_BranchBreakdown</t>
+  </si>
+  <si>
+    <t>SELECT Branch, COUNT(*) AS Count FROM Valid_Claims WHERE Processed_Timestamp = '@RunStart' GROUP BY Branch</t>
+  </si>
+  <si>
+    <t>SQL_AvgClaimAmountValid</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Python_Scripts\generate_excel_summary.py</t>
+  </si>
+  <si>
+    <t>GenerateSummaryPath</t>
+  </si>
+  <si>
+    <t>SELECT (SELECT COUNT(*) FROM Valid_Claims WHERE Processed_Timestamp = '@RunStart') + (SELECT COUNT(*) FROM Invalid_Claims WHERE Processed_Timestamp = '@RunStart') AS TotalClaims</t>
+  </si>
+  <si>
+    <t>SELECT ROUND(AVG(Claim_Amount), 2) AS Average_Claim_Amount FROM Valid_Claims WHERE Processed_Timestamp = '@RunStart'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT COUNT(*) AS ValidClaims FROM Valid_Claims WHERE Processed_Timestamp = '@RunStart' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT COUNT(*) AS InvalidClaims FROM Invalid_Claims WHERE Processed_Timestamp = '@RunStart' </t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\Output\claims_summary.xlsx</t>
+  </si>
+  <si>
+    <t>Subject_SummaryReport</t>
+  </si>
+  <si>
+    <t>Claims Summary Report - Generated Successfully</t>
+  </si>
+  <si>
+    <t>Body_SummaryReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello,
+The claims summary report has been successfully generated and is attached to this email.
+Summary:
+- Report Name: claims_summary.xlsx  
+- Generated On: @Timestamp  
+- Location: Data\Output
+Let me know if you need any adjustments or additional insights.
+Best regards,  
+Robot :)  </t>
   </si>
 </sst>
 </file>
@@ -734,16 +790,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="130.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -798,7 +854,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>44</v>
@@ -816,6 +872,110 @@
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -827,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z53"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1012,226 +1172,189 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>57</v>
+      <c r="B23">
+        <v>1000000</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="180">
       <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="150">
       <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="165">
       <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="180">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="B35" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="180">
       <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="150">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>80</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="225">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="165">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="180">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="210">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="45">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="30">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="225">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="30">
-      <c r="A50" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="30">
-      <c r="A52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1294,10 +1417,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
update workflows and analyze project
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\CIC_Claims_Automation_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0257FB57-651D-4C05-AF0D-A2CE44351981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C0E48A-284E-4C8B-B5F5-F18525C818A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="-13500" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>C:\Users\MorisMwaiWachira\Desktop\MorisMwai_RPA_Assignment\Python_Scripts\hash_policyholder_id.py</t>
-  </si>
-  <si>
-    <t>SQLite_DBPassword</t>
   </si>
   <si>
     <t>DbPath</t>
@@ -793,7 +790,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -853,9 +850,6 @@
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
       <c r="C3" s="4" t="s">
         <v>44</v>
       </c>
@@ -911,7 +905,7 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -927,7 +921,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -935,15 +929,15 @@
         <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -956,26 +950,26 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -1276,18 +1270,18 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="225">
       <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1295,66 +1289,66 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="210">
       <c r="A41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
       <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30">
       <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1415,14 +1409,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>